<commit_message>
update - management commands - seed excel data files
</commit_message>
<xml_diff>
--- a/core/seed_inventories_inventoryadddetail.xlsx
+++ b/core/seed_inventories_inventoryadddetail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan.cheng\Documents\Visual Studio Code\Django\p_sys01_repo01\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D32076-D61E-4FEC-BB69-F3601F4D5567}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86204C1-68BB-4FE6-9EDB-6C349B9E8E38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -887,7 +887,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -916,18 +916,18 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -938,7 +938,7 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>